<commit_message>
Atualizado os gráficos para portugues-br, por que não??
</commit_message>
<xml_diff>
--- a/data/particles.xlsx
+++ b/data/particles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinim\OneDrive\Documentos\Projetos\TCC\fluidization-AE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DE59E6-BA34-43AB-B05D-ED53959800A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82900DEB-78B4-4E92-9C03-EF61931655B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="645" windowWidth="33120" windowHeight="14145" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VIDRO1" sheetId="1" r:id="rId1"/>
@@ -1404,7 +1404,7 @@
                   <c:v>460</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>420</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4400,7 +4400,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4484,7 +4484,7 @@
       </c>
       <c r="K2" s="27">
         <f>1/SUM(H2:H7)</f>
-        <v>736.97616097531431</v>
+        <v>735.35095393292306</v>
       </c>
       <c r="L2" s="25">
         <v>2.5</v>
@@ -4634,12 +4634,12 @@
         <v>15</v>
       </c>
       <c r="G7" s="12">
-        <f t="shared" si="1"/>
-        <v>420</v>
+        <f>E7/2</f>
+        <v>210</v>
       </c>
       <c r="H7" s="22">
         <f t="shared" si="2"/>
-        <v>2.9988904105480976E-6</v>
+        <v>5.9977808210961952E-6</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Atualizado o método para o cálculo do DMS
</commit_message>
<xml_diff>
--- a/data/particles.xlsx
+++ b/data/particles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinim\OneDrive\Documentos\Projetos\TCC\fluidization-AE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82900DEB-78B4-4E92-9C03-EF61931655B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550CDC83-96D1-4EBF-B2B0-DC66BDE91289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2880" yWindow="645" windowWidth="33120" windowHeight="14145" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,8 +37,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Peneiras
 (Mesh)</t>
@@ -166,6 +188,10 @@
   </si>
   <si>
     <t>ESSE QUE TA NO LEITO</t>
+  </si>
+  <si>
+    <t>Massa Total 
+(g)</t>
   </si>
 </sst>
 </file>
@@ -342,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -435,6 +461,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1419,19 +1448,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.049611643691834E-2</c:v>
+                  <c:v>1.0501995379122031E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87.85249457700651</c:v>
+                  <c:v>87.901701323251402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.839619340843887</c:v>
+                  <c:v>11.846250787649652</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11545728080610174</c:v>
+                  <c:v>0.11552194917034235</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1259533972430201</c:v>
+                  <c:v>0.12602394454946439</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1497,19 +1526,19 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.049611643691834E-2</c:v>
+                        <c:v>1.0501995379122031E-2</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>87.85249457700651</c:v>
+                        <c:v>87.901701323251402</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>11.839619340843887</c:v>
+                        <c:v>11.846250787649652</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0.11545728080610174</c:v>
+                        <c:v>0.11552194917034235</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0.1259533972430201</c:v>
+                        <c:v>0.12602394454946439</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4400,7 +4429,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4408,7 +4437,7 @@
     <col min="1" max="7" width="14" customWidth="1"/>
     <col min="8" max="9" width="9.140625"/>
     <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4438,7 +4467,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="K1" s="31" t="s">
         <v>24</v>
@@ -4463,7 +4492,7 @@
       </c>
       <c r="D2" s="3">
         <f>SUM(C3:C7)</f>
-        <v>99.944020712336425</v>
+        <v>99.999999999999972</v>
       </c>
       <c r="E2" s="11">
         <v>1680</v>
@@ -4479,12 +4508,13 @@
         <f>C2/100/G2</f>
         <v>0</v>
       </c>
-      <c r="J2" s="9">
-        <v>1429.1</v>
-      </c>
-      <c r="K2" s="27">
-        <f>1/SUM(H2:H7)</f>
-        <v>735.35095393292306</v>
+      <c r="J2" s="33">
+        <f>SUM(B2:B7)</f>
+        <v>1428.3000000000002</v>
+      </c>
+      <c r="K2" s="27" cm="1">
+        <f t="array" ref="K2">SUM(C2:C7/100)/SUM(H2:H7)</f>
+        <v>734.93930970708413</v>
       </c>
       <c r="L2" s="25">
         <v>2.5</v>
@@ -4499,11 +4529,11 @@
       </c>
       <c r="C3" s="3">
         <f>B3/$J$2*100</f>
-        <v>1.049611643691834E-2</v>
+        <v>1.0501995379122031E-2</v>
       </c>
       <c r="D3" s="3">
         <f>SUM(C4:C7)</f>
-        <v>99.933524595899513</v>
+        <v>99.989498004620856</v>
       </c>
       <c r="E3" s="11">
         <v>1410</v>
@@ -4517,7 +4547,7 @@
       </c>
       <c r="H3" s="21">
         <f>C3/100/G3</f>
-        <v>9.3257365054805334E-8</v>
+        <v>9.3309599103705295E-8</v>
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="24"/>
@@ -4531,11 +4561,11 @@
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:C7" si="0">B4/$J$2*100</f>
-        <v>87.85249457700651</v>
+        <v>87.901701323251402</v>
       </c>
       <c r="D4" s="3">
         <f>SUM(C5:C7)</f>
-        <v>12.081030018893008</v>
+        <v>12.087796681369458</v>
       </c>
       <c r="E4" s="11">
         <v>841</v>
@@ -4544,12 +4574,12 @@
         <v>707</v>
       </c>
       <c r="G4" s="11">
-        <f t="shared" ref="G4:G7" si="1">AVERAGE(E4:F4)</f>
+        <f t="shared" ref="G4:G6" si="1">AVERAGE(E4:F4)</f>
         <v>774</v>
       </c>
       <c r="H4" s="21">
         <f t="shared" ref="H4:H7" si="2">C4/100/G4</f>
-        <v>1.1350451495737276E-3</v>
+        <v>1.1356808956492429E-3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -4561,11 +4591,11 @@
       </c>
       <c r="C5" s="3">
         <f t="shared" si="0"/>
-        <v>11.839619340843887</v>
+        <v>11.846250787649652</v>
       </c>
       <c r="D5" s="3">
         <f>SUM(C6:C7)</f>
-        <v>0.24141067804912184</v>
+        <v>0.24154589371980673</v>
       </c>
       <c r="E5" s="11">
         <v>595</v>
@@ -4579,7 +4609,7 @@
       </c>
       <c r="H5" s="21">
         <f t="shared" si="2"/>
-        <v>2.1624875508390664E-4</v>
+        <v>2.1636987739999364E-4</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -4591,11 +4621,11 @@
       </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>0.11545728080610174</v>
+        <v>0.11552194917034235</v>
       </c>
       <c r="D6" s="3">
         <f>SUM(C7)</f>
-        <v>0.1259533972430201</v>
+        <v>0.12602394454946439</v>
       </c>
       <c r="E6" s="11">
         <v>500</v>
@@ -4609,7 +4639,7 @@
       </c>
       <c r="H6" s="21">
         <f t="shared" si="2"/>
-        <v>2.5099408870891681E-6</v>
+        <v>2.5113467210943988E-6</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -4621,7 +4651,7 @@
       </c>
       <c r="C7" s="7">
         <f t="shared" si="0"/>
-        <v>0.1259533972430201</v>
+        <v>0.12602394454946439</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" ref="D7" si="3">D6-C7</f>
@@ -4639,13 +4669,13 @@
       </c>
       <c r="H7" s="22">
         <f t="shared" si="2"/>
-        <v>5.9977808210961952E-6</v>
+        <v>6.001140216641161E-6</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
+      <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>

</xml_diff>

<commit_message>
Atualizado os gráficos para o estilo do SciencePlots + partícula nova
</commit_message>
<xml_diff>
--- a/data/particles.xlsx
+++ b/data/particles.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinim\OneDrive\Documentos\Projetos\TCC\fluidization-AE\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicampbr-my.sharepoint.com/personal/v195047_m_unicamp_br/Documents/10º Semestre/TCC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550CDC83-96D1-4EBF-B2B0-DC66BDE91289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="335" documentId="11_7F4755BF84DCCE43E268565A8931F45BFA75341E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{995282DA-1277-4E26-A5FA-2AB01E8836F6}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="645" windowWidth="33120" windowHeight="14145" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14085" yWindow="705" windowWidth="23445" windowHeight="14145" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="VIDRO1" sheetId="1" r:id="rId1"/>
-    <sheet name="VIDRO1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="VIDRO1 (3)" sheetId="3" r:id="rId3"/>
+    <sheet name="VIDRO-B" sheetId="1" r:id="rId1"/>
+    <sheet name="VIDRO-B (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="VIDRO-B (3)" sheetId="3" r:id="rId3"/>
+    <sheet name="VIDRO-A" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,30 +38,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>Peneiras
 (Mesh)</t>
@@ -190,8 +169,22 @@
     <t>ESSE QUE TA NO LEITO</t>
   </si>
   <si>
-    <t>Massa Total 
-(g)</t>
+    <t>-35+∞</t>
+  </si>
+  <si>
+    <t>-150+200</t>
+  </si>
+  <si>
+    <t>-200+270</t>
+  </si>
+  <si>
+    <t>-270+325</t>
+  </si>
+  <si>
+    <t>-325+400</t>
+  </si>
+  <si>
+    <t>-400+∞</t>
   </si>
 </sst>
 </file>
@@ -368,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -461,6 +454,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -584,7 +580,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>VIDRO1!$G$2:$G$6</c:f>
+              <c:f>'VIDRO-B'!$G$2:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -608,7 +604,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>VIDRO1!$C$2:$C$6</c:f>
+              <c:f>'VIDRO-B'!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -680,7 +676,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>VIDRO1!$C$2:$C$6</c15:sqref>
+                          <c15:sqref>'VIDRO-B'!$C$2:$C$6</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -994,7 +990,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'VIDRO1 (2)'!$G$2:$G$7</c:f>
+              <c:f>'VIDRO-B (2)'!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1021,7 +1017,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'VIDRO1 (2)'!$C$2:$C$7</c:f>
+              <c:f>'VIDRO-B (2)'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1096,7 +1092,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'VIDRO1 (2)'!$C$2:$C$7</c15:sqref>
+                          <c15:sqref>'VIDRO-B (2)'!$C$2:$C$7</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1413,7 +1409,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'VIDRO1 (3)'!$G$2:$G$7</c:f>
+              <c:f>'VIDRO-B (3)'!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1440,7 +1436,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'VIDRO1 (3)'!$C$2:$C$7</c:f>
+              <c:f>'VIDRO-B (3)'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1515,7 +1511,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'VIDRO1 (3)'!$C$2:$C$7</c15:sqref>
+                          <c15:sqref>'VIDRO-B (3)'!$C$2:$C$7</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1547,6 +1543,416 @@
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-6C3C-42AE-B2FD-845799CF8B9A}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2124086848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2124083488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2124083488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2124086848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Distribuição</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'VIDRO-A'!$G$2:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>89.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'VIDRO-A'!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.37164093767867357</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94339622641509435</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94.139508290451687</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9736992567181244</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.71469411092052604</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3287-4DCD-BD2D-BF6133CA2647}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2124086848"/>
+        <c:axId val="2124083488"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:ln w="38100" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'VIDRO-A'!$C$2:$C$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>0.37164093767867357</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.94339622641509435</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>94.139508290451687</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3.9736992567181244</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.71469411092052604</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-3287-4DCD-BD2D-BF6133CA2647}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1850,6 +2256,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2883,6 +3329,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3523,6 +4485,53 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>529477</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>113180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>535080</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>189380</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{110C128C-3382-4A46-83F9-50FF8CF4401A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4429,7 +5438,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4437,7 +5446,7 @@
     <col min="1" max="7" width="14" customWidth="1"/>
     <col min="8" max="9" width="9.140625"/>
     <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4467,7 +5476,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K1" s="31" t="s">
         <v>24</v>
@@ -4508,13 +5517,13 @@
         <f>C2/100/G2</f>
         <v>0</v>
       </c>
-      <c r="J2" s="33">
+      <c r="J2" s="34">
         <f>SUM(B2:B7)</f>
         <v>1428.3000000000002</v>
       </c>
-      <c r="K2" s="27" cm="1">
-        <f t="array" ref="K2">SUM(C2:C7/100)/SUM(H2:H7)</f>
-        <v>734.93930970708413</v>
+      <c r="K2" s="27">
+        <f>1/SUM(H2:H7)</f>
+        <v>734.93930970708425</v>
       </c>
       <c r="L2" s="25">
         <v>2.5</v>
@@ -4574,7 +5583,7 @@
         <v>707</v>
       </c>
       <c r="G4" s="11">
-        <f t="shared" ref="G4:G6" si="1">AVERAGE(E4:F4)</f>
+        <f t="shared" ref="G4:G7" si="1">AVERAGE(E4:F4)</f>
         <v>774</v>
       </c>
       <c r="H4" s="21">
@@ -4644,7 +5653,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4">
         <v>1.8</v>
@@ -4654,17 +5663,17 @@
         <v>0.12602394454946439</v>
       </c>
       <c r="D7" s="7">
-        <f t="shared" ref="D7" si="3">D6-C7</f>
+        <f>D6-C7</f>
         <v>0</v>
       </c>
       <c r="E7" s="13">
         <v>420</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>15</v>
+      <c r="F7" s="13">
+        <v>0</v>
       </c>
       <c r="G7" s="12">
-        <f>E7/2</f>
+        <f t="shared" si="1"/>
         <v>210</v>
       </c>
       <c r="H7" s="22">
@@ -4675,7 +5684,7 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="1"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -4739,4 +5748,287 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAA294D-62BA-46A0-8D79-A8FA8893C853}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="14" customWidth="1"/>
+    <col min="8" max="9" width="9.140625"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="C2" s="3">
+        <f>B2/$J$2*100</f>
+        <v>0.37164093767867357</v>
+      </c>
+      <c r="D2" s="3">
+        <f>SUM(C3:C6)</f>
+        <v>99.771297884505429</v>
+      </c>
+      <c r="E2" s="11">
+        <v>105</v>
+      </c>
+      <c r="F2" s="11">
+        <v>74</v>
+      </c>
+      <c r="G2" s="11">
+        <f>AVERAGE(E2:F2)</f>
+        <v>89.5</v>
+      </c>
+      <c r="H2" s="21">
+        <f>C2/100/G2</f>
+        <v>4.15241271149356E-5</v>
+      </c>
+      <c r="J2" s="9">
+        <v>349.8</v>
+      </c>
+      <c r="K2" s="27">
+        <f>1/SUM(H2:H6)</f>
+        <v>47.692221548703124</v>
+      </c>
+      <c r="L2" s="25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="C3" s="3">
+        <f>B3/$J$2*100</f>
+        <v>0.94339622641509435</v>
+      </c>
+      <c r="D3" s="3">
+        <f>SUM(C4:C6)</f>
+        <v>98.82790165809034</v>
+      </c>
+      <c r="E3" s="11">
+        <v>74</v>
+      </c>
+      <c r="F3" s="11">
+        <v>53</v>
+      </c>
+      <c r="G3" s="11">
+        <f t="shared" ref="G3:G5" si="0">AVERAGE(E3:F3)</f>
+        <v>63.5</v>
+      </c>
+      <c r="H3" s="21">
+        <f>C3/100/G3</f>
+        <v>1.4856633486851878E-4</v>
+      </c>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="3">
+        <v>329.3</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:C6" si="1">B4/$J$2*100</f>
+        <v>94.139508290451687</v>
+      </c>
+      <c r="D4" s="3">
+        <f>SUM(C5:C6)</f>
+        <v>4.6883933676386507</v>
+      </c>
+      <c r="E4" s="11">
+        <v>53</v>
+      </c>
+      <c r="F4" s="11">
+        <v>44</v>
+      </c>
+      <c r="G4" s="11">
+        <f t="shared" si="0"/>
+        <v>48.5</v>
+      </c>
+      <c r="H4" s="21">
+        <f t="shared" ref="H4:H6" si="2">C4/100/G4</f>
+        <v>1.9410207894938494E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="3">
+        <v>13.9</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="1"/>
+        <v>3.9736992567181244</v>
+      </c>
+      <c r="D5" s="3">
+        <f>SUM(C6:C6)</f>
+        <v>0.71469411092052604</v>
+      </c>
+      <c r="E5" s="11">
+        <v>44</v>
+      </c>
+      <c r="F5" s="11">
+        <v>37</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="0"/>
+        <v>40.5</v>
+      </c>
+      <c r="H5" s="21">
+        <f t="shared" si="2"/>
+        <v>9.8116031030077142E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.71469411092052604</v>
+      </c>
+      <c r="D6" s="4">
+        <f>D5-C6</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
+        <v>37</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <f>E6/2</f>
+        <v>18.5</v>
+      </c>
+      <c r="H6" s="33">
+        <f t="shared" si="2"/>
+        <v>3.8632114103812222E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionada nova partícula + arrumada documentação + função para preparar dados
</commit_message>
<xml_diff>
--- a/data/particles.xlsx
+++ b/data/particles.xlsx
@@ -6,7 +6,7 @@
     <sheet state="visible" name="VIDRO-A1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="VIDRO-B1" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="VIDRO-B2" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="CARVAO" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="VIDRO-B3" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
   <si>
     <t>Peneiras
  (Mesh)</t>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>-48+∞</t>
+  </si>
+  <si>
+    <t>-14+16</t>
+  </si>
+  <si>
+    <t>-48+inf</t>
   </si>
 </sst>
 </file>
@@ -302,11 +308,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2091918899"/>
-        <c:axId val="1519925162"/>
+        <c:axId val="72950865"/>
+        <c:axId val="1973661855"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2091918899"/>
+        <c:axId val="72950865"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -358,10 +364,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1519925162"/>
+        <c:crossAx val="1973661855"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1519925162"/>
+        <c:axId val="1973661855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -436,7 +442,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2091918899"/>
+        <c:crossAx val="72950865"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -506,11 +512,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1855138988"/>
-        <c:axId val="389011526"/>
+        <c:axId val="1506097653"/>
+        <c:axId val="943842835"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1855138988"/>
+        <c:axId val="1506097653"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,10 +568,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="389011526"/>
+        <c:crossAx val="943842835"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="389011526"/>
+        <c:axId val="943842835"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -640,7 +646,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1855138988"/>
+        <c:crossAx val="1506097653"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -710,11 +716,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="69738739"/>
-        <c:axId val="605106079"/>
+        <c:axId val="1429822116"/>
+        <c:axId val="252034413"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="69738739"/>
+        <c:axId val="1429822116"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -766,10 +772,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="605106079"/>
+        <c:crossAx val="252034413"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="605106079"/>
+        <c:axId val="252034413"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -844,7 +850,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69738739"/>
+        <c:crossAx val="1429822116"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -889,26 +895,36 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>CARVAO!$C$1</c:f>
+              <c:f>'VIDRO-B3'!$C$1</c:f>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="434343"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>CARVAO!$G$2:$G$8</c:f>
+              <c:f>'VIDRO-B3'!$G$2:$G$8</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>CARVAO!$C$2:$C$8</c:f>
+              <c:f>'VIDRO-B3'!$C$2:$C$8</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="977685314"/>
-        <c:axId val="1496421374"/>
+        <c:axId val="177793418"/>
+        <c:axId val="1418393387"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="977685314"/>
+        <c:axId val="177793418"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -960,22 +976,85 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1496421374"/>
+        <c:crossAx val="1418393387"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1496421374"/>
+        <c:axId val="1418393387"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
+          <a:ln/>
         </c:spPr>
-        <c:crossAx val="977685314"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="177793418"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2213,62 +2292,72 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8" t="str">
+        <v>29</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="8">
         <f t="shared" ref="C2:C8" si="1">B2/$J$2*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D2" s="7" t="str">
+        <v>0.08212877792</v>
+      </c>
+      <c r="D2" s="16">
         <f>SUM(C3:C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="9" t="str">
+        <v>99.91787122</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1190.0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1000.0</v>
+      </c>
+      <c r="G2" s="9">
         <f t="shared" ref="G2:G8" si="2">AVERAGE(E2:F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H2" s="10" t="str">
+        <v>1095</v>
+      </c>
+      <c r="H2" s="10">
         <f t="shared" ref="H2:H8" si="3">C2/100/G2</f>
-        <v>#DIV/0!</v>
+        <v>0.0000007500345016</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="11">
         <f>SUM(B2:B8)</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="12" t="str">
+        <v>608.8</v>
+      </c>
+      <c r="K2" s="12">
         <f>SUM(C2:C8)/100/SUM(H2:H8)</f>
-        <v>#DIV/0!</v>
+        <v>829.1777913</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="8" t="str">
+        <v>24</v>
+      </c>
+      <c r="B3" s="9">
+        <v>373.3</v>
+      </c>
+      <c r="C3" s="8">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D3" s="9" t="str">
+        <v>61.3173456</v>
+      </c>
+      <c r="D3" s="8">
         <f>SUM(C4:C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E3" s="9" t="str">
+        <v>38.60052562</v>
+      </c>
+      <c r="E3" s="9">
         <f t="shared" ref="E3:E8" si="4">F2</f>
-        <v/>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9" t="str">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="9">
+        <v>841.0</v>
+      </c>
+      <c r="G3" s="9">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H3" s="10" t="str">
+        <v>920.5</v>
+      </c>
+      <c r="H3" s="10">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.0006661308593</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -2276,29 +2365,33 @@
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="8" t="str">
+        <v>25</v>
+      </c>
+      <c r="B4" s="9">
+        <v>233.6</v>
+      </c>
+      <c r="C4" s="8">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D4" s="9" t="str">
+        <v>38.37056505</v>
+      </c>
+      <c r="D4" s="8">
         <f>SUM(C4:C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E4" s="9" t="str">
+        <v>38.60052562</v>
+      </c>
+      <c r="E4" s="9">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="str">
+        <v>841</v>
+      </c>
+      <c r="F4" s="9">
+        <v>595.0</v>
+      </c>
+      <c r="G4" s="9">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H4" s="10" t="str">
+        <v>718</v>
+      </c>
+      <c r="H4" s="10">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.0005344089839</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -2306,29 +2399,33 @@
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="8" t="str">
+        <v>26</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="C5" s="8">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D5" s="9" t="str">
+        <v>0.09855453351</v>
+      </c>
+      <c r="D5" s="8">
         <f>SUM(C5:C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E5" s="9" t="str">
+        <v>0.2299605782</v>
+      </c>
+      <c r="E5" s="9">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9" t="str">
+        <v>595</v>
+      </c>
+      <c r="F5" s="9">
+        <v>500.0</v>
+      </c>
+      <c r="G5" s="9">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H5" s="10" t="str">
+        <v>547.5</v>
+      </c>
+      <c r="H5" s="10">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.000001800082804</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -2336,29 +2433,33 @@
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="8" t="str">
+        <v>27</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C6" s="8">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" s="9" t="str">
+        <v>0.1149802891</v>
+      </c>
+      <c r="D6" s="8">
         <f t="shared" ref="D6:D8" si="5">SUM(C7:C8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" s="9" t="str">
+        <v>0.01642575558</v>
+      </c>
+      <c r="E6" s="9">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9" t="str">
+        <v>500</v>
+      </c>
+      <c r="F6" s="9">
+        <v>420.0</v>
+      </c>
+      <c r="G6" s="9">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H6" s="10" t="str">
+        <v>460</v>
+      </c>
+      <c r="H6" s="10">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.000002499571502</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -2366,29 +2467,33 @@
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8" t="str">
+        <v>17</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="8">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" s="9" t="str">
+        <v>0.01642575558</v>
+      </c>
+      <c r="D7" s="8">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9" t="str">
+        <v>420</v>
+      </c>
+      <c r="F7" s="9">
+        <v>354.0</v>
+      </c>
+      <c r="G7" s="9">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" s="10" t="str">
+        <v>387</v>
+      </c>
+      <c r="H7" s="10">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.0000004244381288</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -2396,29 +2501,33 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14" t="str">
+        <v>30</v>
+      </c>
+      <c r="B8" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="C8" s="14">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="D8" s="13">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E8" s="13" t="str">
+      <c r="E8" s="13">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13" t="str">
+        <v>354</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="13">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="15" t="str">
+        <v>177</v>
+      </c>
+      <c r="H8" s="15">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>

</xml_diff>

<commit_message>
Adicionada a particula de painço e dados de anomalia da particula b3
</commit_message>
<xml_diff>
--- a/data/particles.xlsx
+++ b/data/particles.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="VIDRO-B1" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="VIDRO-B2" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="VIDRO-B3" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="PAINCO" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
   <si>
     <t>Peneiras
  (Mesh)</t>
@@ -116,14 +117,30 @@
   </si>
   <si>
     <t>-48+inf</t>
+  </si>
+  <si>
+    <t>-6+8</t>
+  </si>
+  <si>
+    <t>-8+10</t>
+  </si>
+  <si>
+    <t>-10+12</t>
+  </si>
+  <si>
+    <t>-12+14</t>
+  </si>
+  <si>
+    <t>-20+inf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -206,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -255,6 +272,9 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -308,11 +328,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="72950865"/>
-        <c:axId val="1973661855"/>
+        <c:axId val="2138735094"/>
+        <c:axId val="2045630664"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="72950865"/>
+        <c:axId val="2138735094"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -364,10 +384,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1973661855"/>
+        <c:crossAx val="2045630664"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1973661855"/>
+        <c:axId val="2045630664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -442,7 +462,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72950865"/>
+        <c:crossAx val="2138735094"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -512,11 +532,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1506097653"/>
-        <c:axId val="943842835"/>
+        <c:axId val="1972641799"/>
+        <c:axId val="1491509579"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1506097653"/>
+        <c:axId val="1972641799"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -568,10 +588,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="943842835"/>
+        <c:crossAx val="1491509579"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="943842835"/>
+        <c:axId val="1491509579"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,7 +666,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1506097653"/>
+        <c:crossAx val="1972641799"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -716,11 +736,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1429822116"/>
-        <c:axId val="252034413"/>
+        <c:axId val="1833097166"/>
+        <c:axId val="1865585261"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1429822116"/>
+        <c:axId val="1833097166"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -772,10 +792,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252034413"/>
+        <c:crossAx val="1865585261"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="252034413"/>
+        <c:axId val="1865585261"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,7 +870,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1429822116"/>
+        <c:crossAx val="1833097166"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -920,11 +940,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="177793418"/>
-        <c:axId val="1418393387"/>
+        <c:axId val="695102363"/>
+        <c:axId val="863212183"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="177793418"/>
+        <c:axId val="695102363"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -976,10 +996,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1418393387"/>
+        <c:crossAx val="863212183"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1418393387"/>
+        <c:axId val="863212183"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1054,7 +1074,211 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177793418"/>
+        <c:crossAx val="695102363"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PAINCO!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="434343"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>PAINCO!$G$2:$G$8</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PAINCO!$C$2:$C$8</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1345653943"/>
+        <c:axId val="1184930241"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1345653943"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1184930241"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1184930241"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1345653943"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1183,6 +1407,36 @@
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 4" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4505325" cy="2790825"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 5" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2536,4 +2790,295 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="C2" s="8">
+        <f t="shared" ref="C2:C8" si="1">B2/$J$2*100</f>
+        <v>0.06674453529</v>
+      </c>
+      <c r="D2" s="16">
+        <f>SUM(C3:C8)</f>
+        <v>99.93325546</v>
+      </c>
+      <c r="E2" s="7">
+        <v>3360.0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>2380.0</v>
+      </c>
+      <c r="G2" s="9">
+        <f t="shared" ref="G2:G8" si="2">AVERAGE(E2:F2)</f>
+        <v>2870</v>
+      </c>
+      <c r="H2" s="10">
+        <f t="shared" ref="H2:H8" si="3">C2/100/G2</f>
+        <v>0.0000002325593564</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="11">
+        <f>SUM(B2:B8)</f>
+        <v>599.3</v>
+      </c>
+      <c r="K2" s="12">
+        <f>SUM(C2:C8)/100/SUM(H2:H8)</f>
+        <v>1954.056264</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="9">
+        <v>532.8</v>
+      </c>
+      <c r="C3" s="8">
+        <f t="shared" si="1"/>
+        <v>88.90372101</v>
+      </c>
+      <c r="D3" s="8">
+        <f>SUM(C4:C8)</f>
+        <v>11.02953446</v>
+      </c>
+      <c r="E3" s="9">
+        <f t="shared" ref="E3:E8" si="4">F2</f>
+        <v>2380</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1680.0</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="2"/>
+        <v>2030</v>
+      </c>
+      <c r="H3" s="10">
+        <f t="shared" si="3"/>
+        <v>0.0004379493646</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="9">
+        <v>61.8</v>
+      </c>
+      <c r="C4" s="8">
+        <f t="shared" si="1"/>
+        <v>10.3120307</v>
+      </c>
+      <c r="D4" s="8">
+        <f>SUM(C4:C8)</f>
+        <v>11.02953446</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="4"/>
+        <v>1680</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1410.0</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="2"/>
+        <v>1545</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" si="3"/>
+        <v>0.00006674453529</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="C5" s="8">
+        <f t="shared" si="1"/>
+        <v>0.4171533456</v>
+      </c>
+      <c r="D5" s="8">
+        <f>SUM(C5:C8)</f>
+        <v>0.7175037544</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="4"/>
+        <v>1410</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1190.0</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="2"/>
+        <v>1300</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" si="3"/>
+        <v>0.000003208871889</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="8">
+        <f t="shared" si="1"/>
+        <v>0.1668613382</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" ref="D6:D8" si="5">SUM(C7:C8)</f>
+        <v>0.1334890706</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="4"/>
+        <v>1190</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1000.0</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="2"/>
+        <v>1095</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="3"/>
+        <v>0.000001523847838</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="8">
+        <f t="shared" si="1"/>
+        <v>0.08343066911</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="5"/>
+        <v>0.05005840147</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="F7" s="9">
+        <v>841.0</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="2"/>
+        <v>920.5</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="3"/>
+        <v>0.0000009063625107</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="C8" s="14">
+        <f t="shared" si="1"/>
+        <v>0.05005840147</v>
+      </c>
+      <c r="D8" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="4"/>
+        <v>841</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" si="2"/>
+        <v>420.5</v>
+      </c>
+      <c r="H8" s="15">
+        <f t="shared" si="3"/>
+        <v>0.0000011904495</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionados dados do painço
</commit_message>
<xml_diff>
--- a/data/particles.xlsx
+++ b/data/particles.xlsx
@@ -8,6 +8,7 @@
     <sheet state="visible" name="VIDRO-B2" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="VIDRO-B3" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="PAINCO" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="CARVAO" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="40">
   <si>
     <t>Peneiras
  (Mesh)</t>
@@ -132,6 +133,18 @@
   </si>
   <si>
     <t>-20+inf</t>
+  </si>
+  <si>
+    <t>-7+8</t>
+  </si>
+  <si>
+    <t>-8+9</t>
+  </si>
+  <si>
+    <t>-9+10</t>
+  </si>
+  <si>
+    <t>-16+inf</t>
   </si>
 </sst>
 </file>
@@ -223,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -274,6 +287,15 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -328,11 +350,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2138735094"/>
-        <c:axId val="2045630664"/>
+        <c:axId val="138990197"/>
+        <c:axId val="1254167450"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2138735094"/>
+        <c:axId val="138990197"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -384,10 +406,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2045630664"/>
+        <c:crossAx val="1254167450"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2045630664"/>
+        <c:axId val="1254167450"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -462,7 +484,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2138735094"/>
+        <c:crossAx val="138990197"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -532,11 +554,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1972641799"/>
-        <c:axId val="1491509579"/>
+        <c:axId val="1962929503"/>
+        <c:axId val="1608403407"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1972641799"/>
+        <c:axId val="1962929503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -588,10 +610,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1491509579"/>
+        <c:crossAx val="1608403407"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1491509579"/>
+        <c:axId val="1608403407"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -666,7 +688,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1972641799"/>
+        <c:crossAx val="1962929503"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -736,11 +758,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1833097166"/>
-        <c:axId val="1865585261"/>
+        <c:axId val="1032980651"/>
+        <c:axId val="1636929372"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1833097166"/>
+        <c:axId val="1032980651"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -792,10 +814,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1865585261"/>
+        <c:crossAx val="1636929372"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1865585261"/>
+        <c:axId val="1636929372"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +892,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1833097166"/>
+        <c:crossAx val="1032980651"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -940,11 +962,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="695102363"/>
-        <c:axId val="863212183"/>
+        <c:axId val="174015612"/>
+        <c:axId val="1667450626"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="695102363"/>
+        <c:axId val="174015612"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -996,10 +1018,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="863212183"/>
+        <c:crossAx val="1667450626"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="863212183"/>
+        <c:axId val="1667450626"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1074,7 +1096,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="695102363"/>
+        <c:crossAx val="174015612"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1144,11 +1166,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1345653943"/>
-        <c:axId val="1184930241"/>
+        <c:axId val="1551385636"/>
+        <c:axId val="1272327869"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1345653943"/>
+        <c:axId val="1551385636"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1200,10 +1222,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1184930241"/>
+        <c:crossAx val="1272327869"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1184930241"/>
+        <c:axId val="1272327869"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1278,7 +1300,211 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1345653943"/>
+        <c:crossAx val="1551385636"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CARVAO!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="434343"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>CARVAO!$G$2:$G$8</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CARVAO!$C$2:$C$8</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="76609905"/>
+        <c:axId val="1921131550"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="76609905"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1921131550"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1921131550"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="76609905"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1437,6 +1663,36 @@
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 5" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4505325" cy="2790825"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 6" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3081,4 +3337,295 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="18">
+        <v>34.3</v>
+      </c>
+      <c r="C2" s="8">
+        <f t="shared" ref="C2:C8" si="1">B2/$J$2*100</f>
+        <v>5.731951872</v>
+      </c>
+      <c r="D2" s="16">
+        <f>SUM(C3:C8)</f>
+        <v>94.26804813</v>
+      </c>
+      <c r="E2" s="7">
+        <v>2830.0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>2380.0</v>
+      </c>
+      <c r="G2" s="9">
+        <f t="shared" ref="G2:G8" si="2">AVERAGE(E2:F2)</f>
+        <v>2605</v>
+      </c>
+      <c r="H2" s="10">
+        <f t="shared" ref="H2:H8" si="3">C2/100/G2</f>
+        <v>0.00002200365402</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="19">
+        <f>SUM(B2:B8)</f>
+        <v>598.4</v>
+      </c>
+      <c r="K2" s="12">
+        <f>SUM(C2:C8)/100/SUM(H2:H8)</f>
+        <v>1414.998671</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="17">
+        <v>104.1</v>
+      </c>
+      <c r="C3" s="8">
+        <f t="shared" si="1"/>
+        <v>17.39639037</v>
+      </c>
+      <c r="D3" s="8">
+        <f>SUM(C4:C8)</f>
+        <v>76.87165775</v>
+      </c>
+      <c r="E3" s="9">
+        <f t="shared" ref="E3:E8" si="4">F2</f>
+        <v>2380</v>
+      </c>
+      <c r="F3" s="9">
+        <v>2000.0</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="2"/>
+        <v>2190</v>
+      </c>
+      <c r="H3" s="10">
+        <f t="shared" si="3"/>
+        <v>0.00007943557249</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="17">
+        <v>108.0</v>
+      </c>
+      <c r="C4" s="8">
+        <f t="shared" si="1"/>
+        <v>18.04812834</v>
+      </c>
+      <c r="D4" s="8">
+        <f>SUM(C4:C8)</f>
+        <v>76.87165775</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1680.0</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="2"/>
+        <v>1840</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" si="3"/>
+        <v>0.00009808765403</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="17">
+        <v>164.6</v>
+      </c>
+      <c r="C5" s="8">
+        <f t="shared" si="1"/>
+        <v>27.50668449</v>
+      </c>
+      <c r="D5" s="8">
+        <f>SUM(C5:C8)</f>
+        <v>58.82352941</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="4"/>
+        <v>1680</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1410.0</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="2"/>
+        <v>1545</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" si="3"/>
+        <v>0.0001780367928</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="17">
+        <v>115.0</v>
+      </c>
+      <c r="C6" s="8">
+        <f t="shared" si="1"/>
+        <v>19.21791444</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" ref="D6:D8" si="5">SUM(C7:C8)</f>
+        <v>12.09893048</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="4"/>
+        <v>1410</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1190.0</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="2"/>
+        <v>1300</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="3"/>
+        <v>0.0001478301111</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="17">
+        <v>33.4</v>
+      </c>
+      <c r="C7" s="8">
+        <f t="shared" si="1"/>
+        <v>5.581550802</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="5"/>
+        <v>6.517379679</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="4"/>
+        <v>1190</v>
+      </c>
+      <c r="F7" s="9">
+        <v>1000.0</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="2"/>
+        <v>1095</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="3"/>
+        <v>0.00005097306669</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="20">
+        <v>39.0</v>
+      </c>
+      <c r="C8" s="14">
+        <f t="shared" si="1"/>
+        <v>6.517379679</v>
+      </c>
+      <c r="D8" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="H8" s="15">
+        <f t="shared" si="3"/>
+        <v>0.0001303475936</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refeita a coleta de dados, mudando a posição do sensor PT105
</commit_message>
<xml_diff>
--- a/data/particles.xlsx
+++ b/data/particles.xlsx
@@ -8,6 +8,7 @@
     <sheet state="visible" name="VIDRO-B2" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="VIDRO-B3" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="PAINCO" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="CARVAO" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="40">
   <si>
     <t>Peneiras
  (Mesh)</t>
@@ -132,6 +133,18 @@
   </si>
   <si>
     <t>-20+inf</t>
+  </si>
+  <si>
+    <t>-7+8</t>
+  </si>
+  <si>
+    <t>-8+9</t>
+  </si>
+  <si>
+    <t>-9+10</t>
+  </si>
+  <si>
+    <t>-16+inf</t>
   </si>
 </sst>
 </file>
@@ -223,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -274,6 +287,15 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -328,11 +350,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2138735094"/>
-        <c:axId val="2045630664"/>
+        <c:axId val="887622496"/>
+        <c:axId val="1937963278"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2138735094"/>
+        <c:axId val="887622496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -384,10 +406,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2045630664"/>
+        <c:crossAx val="1937963278"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2045630664"/>
+        <c:axId val="1937963278"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -462,7 +484,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2138735094"/>
+        <c:crossAx val="887622496"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -532,11 +554,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1972641799"/>
-        <c:axId val="1491509579"/>
+        <c:axId val="65244389"/>
+        <c:axId val="593371559"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1972641799"/>
+        <c:axId val="65244389"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -588,10 +610,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1491509579"/>
+        <c:crossAx val="593371559"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1491509579"/>
+        <c:axId val="593371559"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -666,7 +688,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1972641799"/>
+        <c:crossAx val="65244389"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -736,11 +758,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1833097166"/>
-        <c:axId val="1865585261"/>
+        <c:axId val="1139463005"/>
+        <c:axId val="973112810"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1833097166"/>
+        <c:axId val="1139463005"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -792,10 +814,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1865585261"/>
+        <c:crossAx val="973112810"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1865585261"/>
+        <c:axId val="973112810"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +892,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1833097166"/>
+        <c:crossAx val="1139463005"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -940,11 +962,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="695102363"/>
-        <c:axId val="863212183"/>
+        <c:axId val="88310135"/>
+        <c:axId val="1904619162"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="695102363"/>
+        <c:axId val="88310135"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -996,10 +1018,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="863212183"/>
+        <c:crossAx val="1904619162"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="863212183"/>
+        <c:axId val="1904619162"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1074,7 +1096,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="695102363"/>
+        <c:crossAx val="88310135"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1144,11 +1166,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1345653943"/>
-        <c:axId val="1184930241"/>
+        <c:axId val="2056858777"/>
+        <c:axId val="1842805744"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1345653943"/>
+        <c:axId val="2056858777"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1200,10 +1222,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1184930241"/>
+        <c:crossAx val="1842805744"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1184930241"/>
+        <c:axId val="1842805744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1278,7 +1300,211 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1345653943"/>
+        <c:crossAx val="2056858777"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CARVAO!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="434343"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>CARVAO!$G$2:$G$8</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CARVAO!$C$2:$C$8</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="995113840"/>
+        <c:axId val="359783579"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="995113840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="359783579"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="359783579"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="995113840"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1437,6 +1663,36 @@
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 5" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4505325" cy="2790825"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 6" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3081,4 +3337,295 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="18">
+        <v>34.3</v>
+      </c>
+      <c r="C2" s="8">
+        <f t="shared" ref="C2:C8" si="1">B2/$J$2*100</f>
+        <v>5.731951872</v>
+      </c>
+      <c r="D2" s="16">
+        <f>SUM(C3:C8)</f>
+        <v>94.26804813</v>
+      </c>
+      <c r="E2" s="7">
+        <v>2830.0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>2380.0</v>
+      </c>
+      <c r="G2" s="9">
+        <f t="shared" ref="G2:G8" si="2">AVERAGE(E2:F2)</f>
+        <v>2605</v>
+      </c>
+      <c r="H2" s="10">
+        <f t="shared" ref="H2:H8" si="3">C2/100/G2</f>
+        <v>0.00002200365402</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="19">
+        <f>SUM(B2:B8)</f>
+        <v>598.4</v>
+      </c>
+      <c r="K2" s="12">
+        <f>SUM(C2:C8)/100/SUM(H2:H8)</f>
+        <v>1414.998671</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="17">
+        <v>104.1</v>
+      </c>
+      <c r="C3" s="8">
+        <f t="shared" si="1"/>
+        <v>17.39639037</v>
+      </c>
+      <c r="D3" s="8">
+        <f>SUM(C4:C8)</f>
+        <v>76.87165775</v>
+      </c>
+      <c r="E3" s="9">
+        <f t="shared" ref="E3:E8" si="4">F2</f>
+        <v>2380</v>
+      </c>
+      <c r="F3" s="9">
+        <v>2000.0</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="2"/>
+        <v>2190</v>
+      </c>
+      <c r="H3" s="10">
+        <f t="shared" si="3"/>
+        <v>0.00007943557249</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="17">
+        <v>108.0</v>
+      </c>
+      <c r="C4" s="8">
+        <f t="shared" si="1"/>
+        <v>18.04812834</v>
+      </c>
+      <c r="D4" s="8">
+        <f>SUM(C4:C8)</f>
+        <v>76.87165775</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1680.0</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="2"/>
+        <v>1840</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" si="3"/>
+        <v>0.00009808765403</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="17">
+        <v>164.6</v>
+      </c>
+      <c r="C5" s="8">
+        <f t="shared" si="1"/>
+        <v>27.50668449</v>
+      </c>
+      <c r="D5" s="8">
+        <f>SUM(C5:C8)</f>
+        <v>58.82352941</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="4"/>
+        <v>1680</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1410.0</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="2"/>
+        <v>1545</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" si="3"/>
+        <v>0.0001780367928</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="17">
+        <v>115.0</v>
+      </c>
+      <c r="C6" s="8">
+        <f t="shared" si="1"/>
+        <v>19.21791444</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" ref="D6:D8" si="5">SUM(C7:C8)</f>
+        <v>12.09893048</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="4"/>
+        <v>1410</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1190.0</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="2"/>
+        <v>1300</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="3"/>
+        <v>0.0001478301111</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="17">
+        <v>33.4</v>
+      </c>
+      <c r="C7" s="8">
+        <f t="shared" si="1"/>
+        <v>5.581550802</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="5"/>
+        <v>6.517379679</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="4"/>
+        <v>1190</v>
+      </c>
+      <c r="F7" s="9">
+        <v>1000.0</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="2"/>
+        <v>1095</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="3"/>
+        <v>0.00005097306669</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="20">
+        <v>39.0</v>
+      </c>
+      <c r="C8" s="14">
+        <f t="shared" si="1"/>
+        <v>6.517379679</v>
+      </c>
+      <c r="D8" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="H8" s="15">
+        <f t="shared" si="3"/>
+        <v>0.0001303475936</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>